<commit_message>
Final excel created with bug
</commit_message>
<xml_diff>
--- a/data/resumen_downtime.xlsx
+++ b/data/resumen_downtime.xlsx
@@ -74,16 +74,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -455,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +460,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="35" customWidth="1" min="1" max="1"/>
     <col width="40" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -477,79 +474,103 @@
     <row r="2" ht="25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Período analizado:</t>
+          <t>Uptime/Downtime (% General)</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>[PENDIENTE]</t>
+          <t>0.0000%</t>
         </is>
       </c>
     </row>
     <row r="3" ht="25" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Downtime Total:</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>0 segundos</t>
+          <t>Uptime/Downtime (Home+ASH hh:mm:ss)</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Información adicional:</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
-        <is>
-          <t>URL analizada:</t>
-        </is>
-      </c>
-      <c r="B6" s="6" t="inlineStr">
-        <is>
-          <t>https://buenosaires.gob.ar/</t>
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>URLs analizadas:</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Home (main) + ASH</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
-        <is>
-          <t>Total de registros procesados:</t>
-        </is>
-      </c>
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t>4</t>
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Downtime Home (segundos):</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Downtime ASH (segundos):</t>
+        </is>
+      </c>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="inlineStr">
         <is>
           <t>Total downtime (segundos):</t>
         </is>
       </c>
-      <c r="B8" s="6" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+    <row r="10">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>Tiempo total sistema (segundos):</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>2418547</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="inlineStr">
         <is>
           <t>Fecha de generación:</t>
         </is>
       </c>
-      <c r="B9" s="6" t="inlineStr">
-        <is>
-          <t>2025-06-26 16:45:14</t>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>2025-06-27 14:19:46</t>
         </is>
       </c>
     </row>

</xml_diff>